<commit_message>
delete comment in DailyReport-v3.xlsx
</commit_message>
<xml_diff>
--- a/bin/templates/DailyReport-v3.xlsx
+++ b/bin/templates/DailyReport-v3.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerick\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6948"/>
   </bookViews>
   <sheets>
     <sheet name="DailyProductionReport" sheetId="1" r:id="rId1"/>
@@ -21,185 +16,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Jerick</author>
-  </authors>
-  <commentList>
-    <comment ref="J10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jerick:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-"Budget Production Monthly Budget, kWh" / "# of days in a month"</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jerick:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-"Daily Production kWh" * ( "Measured POA Insolation, kWh/m2" / "Daily Budget Energy Production Daily Insolation kWh/m2" )</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jerick:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-"IE POA Insolation kWh/m2" / "# of days in a month"</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jerick:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Summary of the kWh_rec (kWh) from the Gen Meter.  Please take the data from 12:00AM to 11:59PM for 1 day data.
-See Attached Sample.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jerick:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-"Total Energy, kWh" / ("Daily Budget Production, kWh"  * "Total Number of Days")</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Q10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jerick:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-"Month to date Total Energy, kWh" / (("Daily Production, kWh" * "Total Number of Days") * "Weather Performance %" )</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="R10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jerick:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-"Month toDate Total Insolation, kWh/m2" / ("Daily Insolation, kWh/m2" * "Total of Days")</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
@@ -329,7 +145,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="[$-10409]#,##0;\(#,##0\)"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
@@ -337,7 +153,7 @@
     <numFmt numFmtId="167" formatCode="0.0%"/>
     <numFmt numFmtId="168" formatCode="[$-10409]#,##0.0;\(#,##0.0\)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -381,19 +197,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -1112,8 +915,8 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="3" fillId="6" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1460,28 +1263,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y7" sqref="Y7"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.08984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.1796875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.1796875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.21875" style="2" customWidth="1"/>
     <col min="4" max="9" width="13" style="2" customWidth="1"/>
-    <col min="10" max="12" width="12.90625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="19.1796875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="21.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.6328125" style="2" customWidth="1"/>
-    <col min="16" max="18" width="19.1796875" style="2" customWidth="1"/>
+    <col min="10" max="12" width="12.88671875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="19.21875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.6640625" style="2" customWidth="1"/>
+    <col min="16" max="18" width="19.21875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="28.5" customHeight="1">
       <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
@@ -1503,8 +1306,8 @@
       <c r="Q1" s="76"/>
       <c r="R1" s="76"/>
     </row>
-    <row r="2" spans="1:19" ht="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="1.05" customHeight="1"/>
+    <row r="3" spans="1:19" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1512,10 +1315,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="15.75" customHeight="1">
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="18" customHeight="1">
       <c r="A5" s="76" t="s">
         <v>3</v>
       </c>
@@ -1529,8 +1332,8 @@
       <c r="I5" s="1"/>
       <c r="J5" s="33"/>
     </row>
-    <row r="6" spans="1:19" ht="2.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:19" s="9" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="2.7" customHeight="1" thickBot="1"/>
+    <row r="7" spans="1:19" s="9" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A7" s="10"/>
       <c r="B7" s="13"/>
       <c r="C7" s="18"/>
@@ -1560,7 +1363,7 @@
       <c r="Q7" s="81"/>
       <c r="R7" s="81"/>
     </row>
-    <row r="8" spans="1:19" s="3" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" s="3" customFormat="1" ht="12.45" customHeight="1">
       <c r="A8" s="11" t="s">
         <v>5</v>
       </c>
@@ -1614,7 +1417,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="17" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" s="17" customFormat="1" ht="12.45" customHeight="1">
       <c r="A9" s="16"/>
       <c r="B9" s="5"/>
       <c r="C9" s="8"/>
@@ -1662,7 +1465,7 @@
       </c>
       <c r="R9" s="37"/>
     </row>
-    <row r="10" spans="1:19" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="12.45" customHeight="1">
       <c r="A10" s="12">
         <v>1</v>
       </c>
@@ -1722,7 +1525,7 @@
         <v>0.79968379446640314</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="12.45" customHeight="1">
       <c r="A11" s="12">
         <v>2</v>
       </c>
@@ -1782,7 +1585,7 @@
         <v>0.9147613473793732</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="12.45" customHeight="1">
       <c r="A12" s="12">
         <v>3</v>
       </c>
@@ -1842,7 +1645,7 @@
         <v>0.80164682318905078</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="12.45" customHeight="1">
       <c r="A13" s="12">
         <v>4</v>
       </c>
@@ -1902,7 +1705,7 @@
         <v>0.79734894510107157</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="12.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="12.45" customHeight="1" thickBot="1">
       <c r="A14" s="48">
         <v>5</v>
       </c>
@@ -1962,7 +1765,7 @@
         <v>0.73658322353974537</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="13.05" customHeight="1" thickBot="1">
       <c r="A15" s="60"/>
       <c r="B15" s="61" t="s">
         <v>30</v>
@@ -2027,10 +1830,10 @@
       </c>
       <c r="S15" s="72"/>
     </row>
-    <row r="17" spans="1:17" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="12.45" customHeight="1">
       <c r="Q17" s="73"/>
     </row>
-    <row r="21" spans="1:17" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="12.45" customHeight="1">
       <c r="A21" s="70" t="s">
         <v>31</v>
       </c>
@@ -2041,7 +1844,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="12.45" customHeight="1">
       <c r="A22" s="70" t="s">
         <v>32</v>
       </c>
@@ -2074,6 +1877,5 @@
     <ignoredError sqref="Q14 D15:H15 J10:L13 Q11:Q13 Q10 P10:P14 R10:R15 P15:Q15 J14:L14 J15:N15 M14:N14" unlockedFormula="1"/>
     <ignoredError sqref="I15" formula="1" unlockedFormula="1"/>
   </ignoredErrors>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>